<commit_message>
UPDATE: TypeScript SDK facade API - basics (#78)
- workbook operations:
  - cell retrieval
  - sheets access
- sheet operations:
  - access (by index, by name, list all)
  - create
  - delete
  - cell retrieval
- cell operations:
  - get/set value (no typed helpers)
  - get/set formula
</commit_message>
<xml_diff>
--- a/packages/sdk/typescript/examples/node/xlsx/test.xlsx
+++ b/packages/sdk/typescript/examples/node/xlsx/test.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamil/code/EqualToSheets/packages/sdk/wasm/examples/nodejs/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamil/code/EqualToSheets/packages/sdk/typescript/examples/node/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80EE04FC-77F4-374B-8ACF-BBFDD394C81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B094BA-2EB9-F24A-BB35-B7037D896E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10200" yWindow="3820" windowWidth="23020" windowHeight="15420" xr2:uid="{0AB4D8E7-CC82-BB4F-96B9-45ED5D25BB98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Doesitwork " sheetId="3" r:id="rId2"/>
+    <sheet name="Helloworld!" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Input:</t>
   </si>
@@ -45,6 +47,12 @@
   </si>
   <si>
     <t>Percentage:</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Bool:</t>
   </si>
 </sst>
 </file>
@@ -124,11 +132,10 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -446,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BFA89D-FCE2-2349-B528-787E06F39563}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,7 +477,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <f>B1*B1</f>
         <v>9</v>
       </c>
@@ -479,12 +486,52 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <f>B2/B1</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621C23D0-4FF7-EA4D-AECB-43696C13AF39}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9186AE79-2F4E-DC48-9C01-9E8A628DF48E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATE: Move logic from node example to TypeScript SDK tests (#83)
`node` example is now much leaner.
</commit_message>
<xml_diff>
--- a/packages/sdk/typescript/examples/node/xlsx/test.xlsx
+++ b/packages/sdk/typescript/examples/node/xlsx/test.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamil/code/EqualToSheets/packages/sdk/typescript/examples/node/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B094BA-2EB9-F24A-BB35-B7037D896E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D42D63-4308-DF40-AD5C-323F0B9613FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10200" yWindow="3820" windowWidth="23020" windowHeight="15420" xr2:uid="{0AB4D8E7-CC82-BB4F-96B9-45ED5D25BB98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Doesitwork " sheetId="3" r:id="rId2"/>
-    <sheet name="Helloworld!" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Input:</t>
   </si>
@@ -49,10 +47,7 @@
     <t>Percentage:</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Bool:</t>
+    <t>Square &gt;= 17?</t>
   </si>
 </sst>
 </file>
@@ -456,7 +451,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,45 +488,14 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <f>B2&gt;=17</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621C23D0-4FF7-EA4D-AECB-43696C13AF39}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9186AE79-2F4E-DC48-9C01-9E8A628DF48E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>